<commit_message>
Sa Wakas tapos na talaga
</commit_message>
<xml_diff>
--- a/Documentation/Gradebook Format.xlsx
+++ b/Documentation/Gradebook Format.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vibar\source\repos\Grading_System\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CCB139-1754-488E-9906-F3C912EDA213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD002CC1-33E5-473C-803F-AE2FE5238254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{318202C6-DF3C-4E16-A1FD-840DDF55EF30}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quarter 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quarter 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Category:</t>
   </si>
   <si>
-    <t>Task:</t>
-  </si>
-  <si>
     <t>WW:</t>
   </si>
   <si>
@@ -74,9 +72,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Equivalent</t>
-  </si>
-  <si>
     <t>Duran, Josefina Mira</t>
   </si>
   <si>
@@ -90,16 +85,31 @@
   </si>
   <si>
     <t>Gomez, Richard Tila</t>
+  </si>
+  <si>
+    <t>Activity:</t>
+  </si>
+  <si>
+    <t>Total Points:</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -131,19 +141,47 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,24 +192,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,113 +537,107 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="7"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8"/>
-    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2">
-        <f>0.2</f>
+      <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.3</v>
+      <c r="B3" s="13">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="11"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="1" t="s">
+    <row r="6" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="6"/>
+      <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="G6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="7"/>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>7</v>
+      <c r="I6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -606,7 +647,7 @@
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1">
@@ -623,101 +664,329 @@
       <c r="G7" s="1">
         <v>100</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="1">
         <f>SUMIF(5:5, "=QA", 7:7)</f>
         <v>50</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>100</v>
       </c>
-      <c r="K7" s="1">
+      <c r="J7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3">
         <v>10</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>10</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="3">
         <v>20</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="3">
         <v>30</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="3">
         <v>20</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="3">
         <v>20</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="3">
         <v>40</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="4">
+        <f>ROUND((E8*B1)+(G8*B2)+(I8*B3),2)</f>
+        <v>85.64</v>
       </c>
       <c r="D8" s="1">
         <f>SUMIF(5:5, "=WW", 8:8)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
-        <f>D8/D7</f>
-        <v>0</v>
+        <f>ROUND(D8/D7*100,2)</f>
+        <v>85</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUMIF(5:5, "=PT", 8:8)</f>
+        <v>94</v>
+      </c>
+      <c r="G8" s="1">
+        <f>ROUND(F8/F7*100,2)</f>
+        <v>85.45</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUMIF(5:5, "=QA", 8:8)</f>
+        <v>43</v>
+      </c>
+      <c r="I8" s="4">
+        <f>ROUND(H8/H7*100,2)</f>
+        <v>86</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8">
+        <v>25</v>
+      </c>
+      <c r="O8">
+        <v>18</v>
+      </c>
+      <c r="P8">
+        <v>17</v>
+      </c>
+      <c r="Q8">
+        <v>34</v>
+      </c>
+      <c r="R8">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <f>ROUND((E9*B1)+(G9*B2)+(I9*B3),2)</f>
+        <v>82.05</v>
       </c>
       <c r="D9" s="1">
         <f>SUMIF(5:5, "=WW", 9:9)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1">
-        <f>D9/D7</f>
-        <v>0</v>
+        <f>ROUND(D9/D7*100,2)</f>
+        <v>77.5</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUMIF(5:5, "=PT", 9:9)</f>
+        <v>90</v>
+      </c>
+      <c r="G9" s="1">
+        <f>ROUND(F9/F7*100,2)</f>
+        <v>81.819999999999993</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SUMIF(5:5, "=QA", 9:9)</f>
+        <v>42</v>
+      </c>
+      <c r="I9" s="4">
+        <f>H9/H7*100</f>
+        <v>84</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <v>24</v>
+      </c>
+      <c r="O9">
+        <v>17</v>
+      </c>
+      <c r="P9">
+        <v>16</v>
+      </c>
+      <c r="Q9">
+        <v>33</v>
+      </c>
+      <c r="R9">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="4">
+        <f>ROUND((E10*B1)+(G10*B2)+(I10*B3),2)</f>
+        <v>78.180000000000007</v>
       </c>
       <c r="D10" s="1">
         <f>SUMIF(5:5, "=WW", 10:10)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1">
-        <f>D10/D7</f>
-        <v>0</v>
+        <f>ROUND(D10/D7*100,2)</f>
+        <v>70</v>
+      </c>
+      <c r="F10" s="1">
+        <f>SUMIF(5:5, "=PT", 10:10)</f>
+        <v>85</v>
+      </c>
+      <c r="G10" s="1">
+        <f>ROUND(F10/F7*100,2)</f>
+        <v>77.27</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUMIF(5:5, "=QA", 10:10)</f>
+        <v>41</v>
+      </c>
+      <c r="I10" s="4">
+        <f>H10/H7*100</f>
+        <v>82</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>13</v>
+      </c>
+      <c r="N10">
+        <v>23</v>
+      </c>
+      <c r="O10">
+        <v>16</v>
+      </c>
+      <c r="P10">
+        <v>15</v>
+      </c>
+      <c r="Q10">
+        <v>31</v>
+      </c>
+      <c r="R10">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="4">
+        <f>ROUND((E11*B1)+(G11*B2)+(I11*B3),2)</f>
+        <v>74.59</v>
       </c>
       <c r="D11" s="1">
         <f>SUMIF(5:5, "=WW", 11:11)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1">
-        <f>D11/D7</f>
-        <v>0</v>
+        <f>ROUND(D11/D7*100,2)</f>
+        <v>62.5</v>
+      </c>
+      <c r="F11" s="1">
+        <f>SUMIF(5:5, "=PT", 11:11)</f>
+        <v>81</v>
+      </c>
+      <c r="G11" s="1">
+        <f>ROUND(F11/F7*100,2)</f>
+        <v>73.64</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SUMIF(5:5, "=QA", 11:11)</f>
+        <v>40</v>
+      </c>
+      <c r="I11" s="4">
+        <f>H11/H7*100</f>
+        <v>80</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>12</v>
+      </c>
+      <c r="N11">
+        <v>22</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
+        <v>14</v>
+      </c>
+      <c r="Q11">
+        <v>30</v>
+      </c>
+      <c r="R11">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="4">
+        <f>ROUND((E12*B1)+(G12*B2)+(I12*B3),2)</f>
+        <v>66</v>
       </c>
       <c r="D12" s="1">
         <f>SUMIF(5:5, "=WW", 12:12)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1">
-        <f>D12/D7</f>
-        <v>0</v>
+        <f>ROUND(D12/D7*100,2)</f>
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <f>SUMIF(5:5, "=PT", 12:12)</f>
+        <v>77</v>
+      </c>
+      <c r="G12" s="1">
+        <f>ROUND(F12/F7*100,2)</f>
+        <v>70</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SUMIF(5:5, "=QA", 12:12)</f>
+        <v>39</v>
+      </c>
+      <c r="I12" s="4">
+        <f>H12/H7*100</f>
+        <v>78</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>21</v>
+      </c>
+      <c r="O12">
+        <v>14</v>
+      </c>
+      <c r="P12">
+        <v>13</v>
+      </c>
+      <c r="Q12">
+        <v>29</v>
+      </c>
+      <c r="R12">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -726,5 +995,20 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F8 F9:F13 H8" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9A1160-2F0B-4882-A93B-9691C3EFAEBC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>